<commit_message>
Updated Engine List Spreadsheet
</commit_message>
<xml_diff>
--- a/Engine List.xlsx
+++ b/Engine List.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan paplaczyk\Dropbox\GAMES\KSP\Git\ROEngines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\GAMES\KSP\Git\ROEngines\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD60DABA-8DD8-4D08-8BC8-3E85483C9360}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18000" windowHeight="9360" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Remove" sheetId="1" r:id="rId1"/>
     <sheet name="List" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Other Parts" sheetId="3" r:id="rId3"/>
+    <sheet name="RaiderNick" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="379">
   <si>
     <t>engineType</t>
   </si>
@@ -652,9 +654,6 @@
     <t>R42</t>
   </si>
   <si>
-    <t>Kick Motor</t>
-  </si>
-  <si>
     <t>R40</t>
   </si>
   <si>
@@ -979,9 +978,6 @@
     <t>BabySergeant</t>
   </si>
   <si>
-    <t>FASA, BDB</t>
-  </si>
-  <si>
     <t>FASAExplorerSgt11Dec</t>
   </si>
   <si>
@@ -992,12 +988,189 @@
   </si>
   <si>
     <t>rn_junoii_sgt_3_dec</t>
+  </si>
+  <si>
+    <t>aerobee300_srb</t>
+  </si>
+  <si>
+    <t>aerobee170_srb</t>
+  </si>
+  <si>
+    <t>aerobee150_srb</t>
+  </si>
+  <si>
+    <t>junoii_sgt</t>
+  </si>
+  <si>
+    <t>junoii_sgt_3</t>
+  </si>
+  <si>
+    <t>junoii_sgt_3_dec</t>
+  </si>
+  <si>
+    <t>junoii_sgt_11</t>
+  </si>
+  <si>
+    <t>junoii_sgt_11_dec</t>
+  </si>
+  <si>
+    <t>thor_star37d</t>
+  </si>
+  <si>
+    <t>srmu_mb</t>
+  </si>
+  <si>
+    <t>srmu_nc</t>
+  </si>
+  <si>
+    <t>ua1207</t>
+  </si>
+  <si>
+    <t>ua1207_nc</t>
+  </si>
+  <si>
+    <t>Baby Sergeant</t>
+  </si>
+  <si>
+    <t>3x Decoupler</t>
+  </si>
+  <si>
+    <t>Baby Sergeant x3</t>
+  </si>
+  <si>
+    <t>11x Decoupler</t>
+  </si>
+  <si>
+    <t>Baby Sergeant x11</t>
+  </si>
+  <si>
+    <t>thor_star20</t>
+  </si>
+  <si>
+    <t>TE-M-640-1 Star 20</t>
+  </si>
+  <si>
+    <t>Thor-Burner 1</t>
+  </si>
+  <si>
+    <t>TE-M-364-3 Star-37D</t>
+  </si>
+  <si>
+    <t>Delta J-M</t>
+  </si>
+  <si>
+    <t>USA1207 SRM</t>
+  </si>
+  <si>
+    <t>ua1205 (1205)</t>
+  </si>
+  <si>
+    <t>ua1206 (1206)</t>
+  </si>
+  <si>
+    <t>USA1207 Nosecone</t>
+  </si>
+  <si>
+    <t>ua1205_nc (1205)</t>
+  </si>
+  <si>
+    <t>ua1206_nc (1205)</t>
+  </si>
+  <si>
+    <t>SRMU Nosecone</t>
+  </si>
+  <si>
+    <t>2.5KS-18000</t>
+  </si>
+  <si>
+    <t>M5E1 Nike</t>
+  </si>
+  <si>
+    <t>1.8KS-7800</t>
+  </si>
+  <si>
+    <t>FASA, BDB, RN</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>Maneuver Motor (Cassini)</t>
+  </si>
+  <si>
+    <t>Niche Parts</t>
+  </si>
+  <si>
+    <t>NicheParts</t>
+  </si>
+  <si>
+    <t>BE-3</t>
+  </si>
+  <si>
+    <t>Addon</t>
+  </si>
+  <si>
+    <t>Rutherford</t>
+  </si>
+  <si>
+    <t>RutherfordVac</t>
+  </si>
+  <si>
+    <t>400N</t>
+  </si>
+  <si>
+    <t>S-400 Maneuvers (Galileo, Venus Express)</t>
+  </si>
+  <si>
+    <t>MR80B</t>
+  </si>
+  <si>
+    <t>Mars Landing Engine (Curiosity)</t>
+  </si>
+  <si>
+    <t>MR80TDE</t>
+  </si>
+  <si>
+    <t>Viking Landers</t>
+  </si>
+  <si>
+    <t>MR104</t>
+  </si>
+  <si>
+    <t>Voyager 1-2</t>
+  </si>
+  <si>
+    <t>MR107</t>
+  </si>
+  <si>
+    <t>Probes, Landers (Phoenix Mars, Mars Polar)</t>
+  </si>
+  <si>
+    <t>Star-5D</t>
+  </si>
+  <si>
+    <t>Pathfinder Lander</t>
+  </si>
+  <si>
+    <t>Star-8</t>
+  </si>
+  <si>
+    <t>MER (Spirit / Opportunity Landers)</t>
+  </si>
+  <si>
+    <t>LEROS1b</t>
+  </si>
+  <si>
+    <t>Satellite Engines</t>
+  </si>
+  <si>
+    <t>R4D11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1082,34 +1255,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K182" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:K182">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Solid"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:K194" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:K194" xr:uid="{02A2150E-C9F6-46C9-AAD1-F16658D4FC30}"/>
   <sortState ref="A2:K182">
     <sortCondition ref="A1:A182"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" name="Engine"/>
-    <tableColumn id="2" name="Type"/>
-    <tableColumn id="3" name="Mods"/>
-    <tableColumn id="4" name="Notes"/>
-    <tableColumn id="5" name="Craft"/>
-    <tableColumn id="11" name="Year"/>
-    <tableColumn id="6" name="Include" dataDxfId="4"/>
-    <tableColumn id="7" name="Mod Choice" dataDxfId="3"/>
-    <tableColumn id="8" name="Complete" dataDxfId="2"/>
-    <tableColumn id="9" name="Added to RP1" dataDxfId="1"/>
-    <tableColumn id="10" name="REMOVE" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Engine"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Mods"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Notes"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Craft"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Year"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Include" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Mod Choice" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complete" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Added to RP1" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="REMOVE" dataDxfId="0">
       <calculatedColumnFormula>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A2&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1379,7 +1541,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1639,11 +1801,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K182"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,7 +1840,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>66</v>
@@ -1690,13 +1852,13 @@
         <v>67</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1729,7 +1891,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[A-4]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1762,7 +1924,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[Aerobee]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -1780,7 +1942,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1813,7 +1975,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[Agena]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1831,7 +1993,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1864,7 +2026,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[AJ10_137]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1897,7 +2059,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[AJ10_190]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -1905,7 +2067,7 @@
         <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F9">
         <v>1972</v>
@@ -1914,7 +2076,7 @@
         <v>70</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>70</v>
@@ -1927,7 +2089,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[AJ10_Adv]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1935,7 +2097,7 @@
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F10">
         <v>1959</v>
@@ -1957,7 +2119,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[AJ10_Early]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1965,7 +2127,7 @@
         <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F11">
         <v>1960</v>
@@ -2053,7 +2215,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[AJ260SL]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -2077,7 +2239,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2101,7 +2263,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -2125,7 +2287,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2149,7 +2311,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2170,7 +2332,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2197,7 +2359,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2224,7 +2386,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -2251,7 +2413,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2278,7 +2440,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2305,7 +2467,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2326,7 +2488,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -2347,7 +2509,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -2370,7 +2532,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B27" t="s">
         <v>31</v>
@@ -2401,7 +2563,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[BabySergeant]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2419,7 +2581,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>80</v>
       </c>
@@ -2434,7 +2596,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>117</v>
       </c>
@@ -2457,7 +2619,7 @@
         <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>317</v>
+        <v>353</v>
       </c>
       <c r="E31" t="s">
         <v>116</v>
@@ -2469,7 +2631,7 @@
         <v>70</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>32</v>
+        <v>354</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>70</v>
@@ -2482,7 +2644,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[Castor-1]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>102</v>
       </c>
@@ -2500,7 +2662,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -2518,7 +2680,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>107</v>
       </c>
@@ -2533,7 +2695,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -2548,7 +2710,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -2566,7 +2728,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>112</v>
       </c>
@@ -2584,7 +2746,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>110</v>
       </c>
@@ -2602,7 +2764,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -2620,7 +2782,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -2641,7 +2803,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>99</v>
       </c>
@@ -2662,7 +2824,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -2686,7 +2848,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -2719,7 +2881,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[F1]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -2737,7 +2899,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>119</v>
       </c>
@@ -2755,7 +2917,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>148</v>
       </c>
@@ -2773,7 +2935,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>146</v>
       </c>
@@ -2791,7 +2953,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>144</v>
       </c>
@@ -2812,7 +2974,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>143</v>
       </c>
@@ -2833,7 +2995,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -2854,7 +3016,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>139</v>
       </c>
@@ -2875,7 +3037,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>137</v>
       </c>
@@ -2893,7 +3055,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>135</v>
       </c>
@@ -2911,7 +3073,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -2944,7 +3106,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[H1]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>132</v>
       </c>
@@ -2959,7 +3121,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>130</v>
       </c>
@@ -2974,7 +3136,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>17</v>
       </c>
@@ -3001,7 +3163,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[J2]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>129</v>
       </c>
@@ -3016,7 +3178,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -3043,7 +3205,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[J2X]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>126</v>
       </c>
@@ -3070,7 +3232,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>128</v>
       </c>
@@ -3097,7 +3259,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>125</v>
       </c>
@@ -3115,7 +3277,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -3133,7 +3295,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>122</v>
       </c>
@@ -3145,7 +3307,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>121</v>
       </c>
@@ -3157,7 +3319,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>173</v>
       </c>
@@ -3178,7 +3340,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>170</v>
       </c>
@@ -3196,7 +3358,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>168</v>
       </c>
@@ -3211,7 +3373,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>166</v>
       </c>
@@ -3226,7 +3388,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>165</v>
       </c>
@@ -3250,7 +3412,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>163</v>
       </c>
@@ -3274,7 +3436,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -3307,7 +3469,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[LR101]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -3340,7 +3502,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[LR105]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>15</v>
       </c>
@@ -3373,7 +3535,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[LR79]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>159</v>
       </c>
@@ -3391,7 +3553,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>158</v>
       </c>
@@ -3412,7 +3574,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>157</v>
       </c>
@@ -3427,7 +3589,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -3460,7 +3622,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[LR89]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>155</v>
       </c>
@@ -3481,7 +3643,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>153</v>
       </c>
@@ -3502,7 +3664,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>151</v>
       </c>
@@ -3520,7 +3682,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>149</v>
       </c>
@@ -3547,7 +3709,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>185</v>
       </c>
@@ -3562,7 +3724,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>184</v>
       </c>
@@ -3577,7 +3739,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>183</v>
       </c>
@@ -3592,7 +3754,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>182</v>
       </c>
@@ -3607,7 +3769,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -3640,7 +3802,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[NAA75_110]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>178</v>
       </c>
@@ -3652,7 +3814,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>177</v>
       </c>
@@ -3664,7 +3826,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>180</v>
       </c>
@@ -3676,7 +3838,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>179</v>
       </c>
@@ -3696,7 +3858,7 @@
         <v>31</v>
       </c>
       <c r="C92" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E92" t="s">
         <v>176</v>
@@ -3708,7 +3870,7 @@
         <v>70</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>70</v>
@@ -3721,7 +3883,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[Nike-M5E1]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>190</v>
       </c>
@@ -3739,9 +3901,9 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B94" t="s">
         <v>65</v>
@@ -3754,7 +3916,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>193</v>
       </c>
@@ -3772,7 +3934,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>192</v>
       </c>
@@ -3790,21 +3952,21 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>213</v>
+      </c>
+      <c r="B97" t="s">
         <v>214</v>
-      </c>
-      <c r="B97" t="s">
-        <v>215</v>
       </c>
       <c r="K97" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A97&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B98" t="s">
         <v>81</v>
@@ -3814,9 +3976,9 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B99" t="s">
         <v>81</v>
@@ -3826,9 +3988,9 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B100" t="s">
         <v>81</v>
@@ -3838,40 +4000,58 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>208</v>
+      </c>
+      <c r="B101" t="s">
+        <v>65</v>
+      </c>
+      <c r="C101" t="s">
+        <v>356</v>
+      </c>
+      <c r="D101" t="s">
         <v>209</v>
-      </c>
-      <c r="B101" t="s">
-        <v>65</v>
-      </c>
-      <c r="D101" t="s">
-        <v>210</v>
       </c>
       <c r="E101" t="s">
         <v>73</v>
       </c>
+      <c r="G101" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>357</v>
+      </c>
       <c r="K101" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A101&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>207</v>
       </c>
       <c r="B102" t="s">
         <v>65</v>
       </c>
+      <c r="C102" t="s">
+        <v>356</v>
+      </c>
       <c r="E102" t="s">
-        <v>208</v>
+        <v>355</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>357</v>
       </c>
       <c r="K102" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A102&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -3895,7 +4075,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>199</v>
       </c>
@@ -3916,7 +4096,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -3937,7 +4117,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>194</v>
       </c>
@@ -3958,9 +4138,9 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B107" t="s">
         <v>65</v>
@@ -3969,7 +4149,7 @@
         <v>195</v>
       </c>
       <c r="E107" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F107">
         <v>2013</v>
@@ -3979,15 +4159,15 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>222</v>
+      </c>
+      <c r="B108" t="s">
+        <v>65</v>
+      </c>
+      <c r="E108" t="s">
         <v>223</v>
-      </c>
-      <c r="B108" t="s">
-        <v>65</v>
-      </c>
-      <c r="E108" t="s">
-        <v>224</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>70</v>
@@ -3997,84 +4177,84 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>219</v>
+      </c>
+      <c r="B109" t="s">
+        <v>65</v>
+      </c>
+      <c r="E109" t="s">
         <v>220</v>
-      </c>
-      <c r="B109" t="s">
-        <v>65</v>
-      </c>
-      <c r="E109" t="s">
-        <v>221</v>
       </c>
       <c r="K109" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A109&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>217</v>
+      </c>
+      <c r="B110" t="s">
+        <v>65</v>
+      </c>
+      <c r="D110" t="s">
         <v>218</v>
-      </c>
-      <c r="B110" t="s">
-        <v>65</v>
-      </c>
-      <c r="D110" t="s">
-        <v>219</v>
       </c>
       <c r="K110" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A110&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B111" t="s">
         <v>65</v>
       </c>
       <c r="E111" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K111" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A111&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B112" t="s">
         <v>65</v>
       </c>
       <c r="E112" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K112" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A112&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B113" t="s">
         <v>65</v>
       </c>
       <c r="E113" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K113" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A113&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B114" t="s">
         <v>65</v>
@@ -4083,16 +4263,16 @@
         <v>195</v>
       </c>
       <c r="E114" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K114" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A114&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B115" t="s">
         <v>65</v>
@@ -4102,9 +4282,9 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B116" t="s">
         <v>81</v>
@@ -4114,7 +4294,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>12</v>
       </c>
@@ -4144,7 +4324,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[RD100]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -4177,7 +4357,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[RD107-117]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>10</v>
       </c>
@@ -4210,9 +4390,9 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[RD108-118]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B120" t="s">
         <v>65</v>
@@ -4225,7 +4405,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>8</v>
       </c>
@@ -4236,7 +4416,7 @@
         <v>72</v>
       </c>
       <c r="E121" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>70</v>
@@ -4255,7 +4435,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[RD170]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>7</v>
       </c>
@@ -4285,7 +4465,7 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[RD180]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -4296,7 +4476,7 @@
         <v>72</v>
       </c>
       <c r="E123" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>70</v>
@@ -4315,52 +4495,52 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[RD191]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>237</v>
+      </c>
+      <c r="B124" t="s">
+        <v>65</v>
+      </c>
+      <c r="E124" t="s">
         <v>238</v>
-      </c>
-      <c r="B124" t="s">
-        <v>65</v>
-      </c>
-      <c r="E124" t="s">
-        <v>239</v>
       </c>
       <c r="K124" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A124&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>235</v>
+      </c>
+      <c r="B125" t="s">
+        <v>65</v>
+      </c>
+      <c r="D125" t="s">
         <v>236</v>
-      </c>
-      <c r="B125" t="s">
-        <v>65</v>
-      </c>
-      <c r="D125" t="s">
-        <v>237</v>
       </c>
       <c r="K125" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A125&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>233</v>
+      </c>
+      <c r="B126" t="s">
+        <v>65</v>
+      </c>
+      <c r="E126" t="s">
         <v>234</v>
-      </c>
-      <c r="B126" t="s">
-        <v>65</v>
-      </c>
-      <c r="E126" t="s">
-        <v>235</v>
       </c>
       <c r="K126" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A126&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>202</v>
       </c>
@@ -4375,7 +4555,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>200</v>
       </c>
@@ -4393,37 +4573,37 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B129" t="s">
         <v>65</v>
       </c>
       <c r="E129" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K129" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A129&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>229</v>
+      </c>
+      <c r="B130" t="s">
+        <v>65</v>
+      </c>
+      <c r="E130" t="s">
         <v>230</v>
-      </c>
-      <c r="B130" t="s">
-        <v>65</v>
-      </c>
-      <c r="E130" t="s">
-        <v>231</v>
       </c>
       <c r="K130" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A130&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>203</v>
       </c>
@@ -4441,9 +4621,9 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B132" t="s">
         <v>65</v>
@@ -4456,9 +4636,9 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B133" t="s">
         <v>65</v>
@@ -4467,7 +4647,7 @@
         <v>195</v>
       </c>
       <c r="E133" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F133">
         <v>1964</v>
@@ -4477,9 +4657,9 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B134" t="s">
         <v>65</v>
@@ -4488,7 +4668,7 @@
         <v>195</v>
       </c>
       <c r="E134" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F134">
         <v>1964</v>
@@ -4498,9 +4678,9 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B135" t="s">
         <v>31</v>
@@ -4519,7 +4699,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>5</v>
       </c>
@@ -4530,7 +4710,7 @@
         <v>72</v>
       </c>
       <c r="E136" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>70</v>
@@ -4549,22 +4729,22 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[RL10]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>245</v>
+      </c>
+      <c r="B137" t="s">
+        <v>65</v>
+      </c>
+      <c r="E137" t="s">
         <v>246</v>
-      </c>
-      <c r="B137" t="s">
-        <v>65</v>
-      </c>
-      <c r="E137" t="s">
-        <v>247</v>
       </c>
       <c r="K137" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A137&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>3</v>
       </c>
@@ -4594,24 +4774,24 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[RS68]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>270</v>
+      </c>
+      <c r="B139" t="s">
+        <v>65</v>
+      </c>
+      <c r="E139" t="s">
         <v>271</v>
-      </c>
-      <c r="B139" t="s">
-        <v>65</v>
-      </c>
-      <c r="E139" t="s">
-        <v>272</v>
       </c>
       <c r="K139" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A139&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B140" t="s">
         <v>31</v>
@@ -4630,15 +4810,15 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>267</v>
+      </c>
+      <c r="B141" t="s">
+        <v>31</v>
+      </c>
+      <c r="E141" t="s">
         <v>268</v>
-      </c>
-      <c r="B141" t="s">
-        <v>31</v>
-      </c>
-      <c r="E141" t="s">
-        <v>269</v>
       </c>
       <c r="F141">
         <v>2012</v>
@@ -4648,9 +4828,9 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B142" t="s">
         <v>31</v>
@@ -4669,15 +4849,15 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>264</v>
+      </c>
+      <c r="B143" t="s">
+        <v>65</v>
+      </c>
+      <c r="E143" t="s">
         <v>265</v>
-      </c>
-      <c r="B143" t="s">
-        <v>65</v>
-      </c>
-      <c r="E143" t="s">
-        <v>266</v>
       </c>
       <c r="F143">
         <v>1953</v>
@@ -4690,15 +4870,15 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>262</v>
+      </c>
+      <c r="B144" t="s">
+        <v>65</v>
+      </c>
+      <c r="E144" t="s">
         <v>263</v>
-      </c>
-      <c r="B144" t="s">
-        <v>65</v>
-      </c>
-      <c r="E144" t="s">
-        <v>264</v>
       </c>
       <c r="F144">
         <v>2000</v>
@@ -4708,15 +4888,15 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>260</v>
+      </c>
+      <c r="B145" t="s">
+        <v>65</v>
+      </c>
+      <c r="E145" t="s">
         <v>261</v>
-      </c>
-      <c r="B145" t="s">
-        <v>65</v>
-      </c>
-      <c r="E145" t="s">
-        <v>262</v>
       </c>
       <c r="F145">
         <v>2000</v>
@@ -4726,15 +4906,15 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
+        <v>258</v>
+      </c>
+      <c r="B146" t="s">
+        <v>65</v>
+      </c>
+      <c r="D146" t="s">
         <v>259</v>
-      </c>
-      <c r="B146" t="s">
-        <v>65</v>
-      </c>
-      <c r="D146" t="s">
-        <v>260</v>
       </c>
       <c r="E146" t="s">
         <v>95</v>
@@ -4747,9 +4927,9 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B147" t="s">
         <v>81</v>
@@ -4759,15 +4939,15 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>255</v>
+      </c>
+      <c r="B148" t="s">
+        <v>31</v>
+      </c>
+      <c r="E148" t="s">
         <v>256</v>
-      </c>
-      <c r="B148" t="s">
-        <v>31</v>
-      </c>
-      <c r="E148" t="s">
-        <v>257</v>
       </c>
       <c r="F148">
         <v>1989</v>
@@ -4780,7 +4960,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>4</v>
       </c>
@@ -4810,9 +4990,9 @@
         <v>!PART:HAS[~name[ROE-*]&amp;#engineType[SSME]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B150" t="s">
         <v>31</v>
@@ -4822,9 +5002,9 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B151" t="s">
         <v>31</v>
@@ -4834,9 +5014,9 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B152" t="s">
         <v>31</v>
@@ -4849,9 +5029,9 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B153" t="s">
         <v>31</v>
@@ -4861,9 +5041,9 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B154" t="s">
         <v>31</v>
@@ -4873,9 +5053,9 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B155" t="s">
         <v>31</v>
@@ -4885,9 +5065,9 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B156" t="s">
         <v>31</v>
@@ -4897,9 +5077,9 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B157" t="s">
         <v>31</v>
@@ -4909,9 +5089,9 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B158" t="s">
         <v>31</v>
@@ -4921,9 +5101,9 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B159" t="s">
         <v>31</v>
@@ -4933,9 +5113,9 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B160" t="s">
         <v>31</v>
@@ -4948,9 +5128,9 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B161" t="s">
         <v>31</v>
@@ -4963,9 +5143,9 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B162" t="s">
         <v>31</v>
@@ -4978,9 +5158,9 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B163" t="s">
         <v>31</v>
@@ -4993,9 +5173,9 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B164" t="s">
         <v>31</v>
@@ -5008,9 +5188,9 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B165" t="s">
         <v>31</v>
@@ -5023,9 +5203,9 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B166" t="s">
         <v>31</v>
@@ -5038,9 +5218,9 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B167" t="s">
         <v>31</v>
@@ -5053,9 +5233,9 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B168" t="s">
         <v>31</v>
@@ -5068,9 +5248,9 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B169" t="s">
         <v>65</v>
@@ -5079,7 +5259,7 @@
         <v>72</v>
       </c>
       <c r="E169" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G169" s="1" t="s">
         <v>70</v>
@@ -5092,24 +5272,24 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>303</v>
+      </c>
+      <c r="B170" t="s">
+        <v>65</v>
+      </c>
+      <c r="E170" t="s">
         <v>304</v>
-      </c>
-      <c r="B170" t="s">
-        <v>65</v>
-      </c>
-      <c r="E170" t="s">
-        <v>305</v>
       </c>
       <c r="K170" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A170&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B171" t="s">
         <v>31</v>
@@ -5125,15 +5305,15 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
+        <v>300</v>
+      </c>
+      <c r="B172" t="s">
+        <v>31</v>
+      </c>
+      <c r="E172" t="s">
         <v>301</v>
-      </c>
-      <c r="B172" t="s">
-        <v>31</v>
-      </c>
-      <c r="E172" t="s">
-        <v>302</v>
       </c>
       <c r="F172">
         <v>1965</v>
@@ -5146,15 +5326,15 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>298</v>
+      </c>
+      <c r="B173" t="s">
+        <v>31</v>
+      </c>
+      <c r="E173" t="s">
         <v>299</v>
-      </c>
-      <c r="B173" t="s">
-        <v>31</v>
-      </c>
-      <c r="E173" t="s">
-        <v>300</v>
       </c>
       <c r="F173">
         <v>1989</v>
@@ -5167,9 +5347,9 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B174" t="s">
         <v>65</v>
@@ -5185,39 +5365,39 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>295</v>
+      </c>
+      <c r="B175" t="s">
+        <v>65</v>
+      </c>
+      <c r="E175" t="s">
         <v>296</v>
-      </c>
-      <c r="B175" t="s">
-        <v>65</v>
-      </c>
-      <c r="E175" t="s">
-        <v>297</v>
       </c>
       <c r="K175" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A175&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>293</v>
+      </c>
+      <c r="B176" t="s">
+        <v>65</v>
+      </c>
+      <c r="E176" t="s">
         <v>294</v>
-      </c>
-      <c r="B176" t="s">
-        <v>65</v>
-      </c>
-      <c r="E176" t="s">
-        <v>295</v>
       </c>
       <c r="K176" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A176&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B177" t="s">
         <v>31</v>
@@ -5233,9 +5413,9 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B178" t="s">
         <v>65</v>
@@ -5254,27 +5434,27 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B179" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K179" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A179&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>288</v>
+      </c>
+      <c r="B180" t="s">
+        <v>65</v>
+      </c>
+      <c r="E180" t="s">
         <v>289</v>
-      </c>
-      <c r="B180" t="s">
-        <v>65</v>
-      </c>
-      <c r="E180" t="s">
-        <v>290</v>
       </c>
       <c r="F180">
         <v>0</v>
@@ -5284,15 +5464,15 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>286</v>
+      </c>
+      <c r="B181" t="s">
+        <v>65</v>
+      </c>
+      <c r="E181" t="s">
         <v>287</v>
-      </c>
-      <c r="B181" t="s">
-        <v>65</v>
-      </c>
-      <c r="E181" t="s">
-        <v>288</v>
       </c>
       <c r="F181">
         <v>1959</v>
@@ -5302,18 +5482,255 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>284</v>
+      </c>
+      <c r="B182" t="s">
+        <v>65</v>
+      </c>
+      <c r="E182" t="s">
         <v>285</v>
-      </c>
-      <c r="B182" t="s">
-        <v>65</v>
-      </c>
-      <c r="E182" t="s">
-        <v>286</v>
       </c>
       <c r="K182" s="1" t="str">
         <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A182&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>358</v>
+      </c>
+      <c r="B183" t="s">
+        <v>359</v>
+      </c>
+      <c r="C183" t="s">
+        <v>356</v>
+      </c>
+      <c r="K183" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A183&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>360</v>
+      </c>
+      <c r="B184" t="s">
+        <v>359</v>
+      </c>
+      <c r="C184" t="s">
+        <v>356</v>
+      </c>
+      <c r="K184" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A184&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>361</v>
+      </c>
+      <c r="B185" t="s">
+        <v>359</v>
+      </c>
+      <c r="C185" t="s">
+        <v>356</v>
+      </c>
+      <c r="K185" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A185&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>362</v>
+      </c>
+      <c r="B186" t="s">
+        <v>359</v>
+      </c>
+      <c r="C186" t="s">
+        <v>356</v>
+      </c>
+      <c r="E186" t="s">
+        <v>363</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H186" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="K186" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A186&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>364</v>
+      </c>
+      <c r="B187" t="s">
+        <v>359</v>
+      </c>
+      <c r="C187" t="s">
+        <v>356</v>
+      </c>
+      <c r="E187" t="s">
+        <v>365</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H187" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="K187" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A187&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>366</v>
+      </c>
+      <c r="B188" t="s">
+        <v>359</v>
+      </c>
+      <c r="C188" t="s">
+        <v>356</v>
+      </c>
+      <c r="E188" t="s">
+        <v>367</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="K188" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A188&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>368</v>
+      </c>
+      <c r="B189" t="s">
+        <v>359</v>
+      </c>
+      <c r="C189" t="s">
+        <v>356</v>
+      </c>
+      <c r="E189" t="s">
+        <v>369</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H189" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="K189" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A189&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>370</v>
+      </c>
+      <c r="B190" t="s">
+        <v>359</v>
+      </c>
+      <c r="C190" t="s">
+        <v>356</v>
+      </c>
+      <c r="E190" t="s">
+        <v>371</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H190" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="K190" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A190&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>372</v>
+      </c>
+      <c r="B191" t="s">
+        <v>359</v>
+      </c>
+      <c r="C191" t="s">
+        <v>356</v>
+      </c>
+      <c r="E191" t="s">
+        <v>373</v>
+      </c>
+      <c r="K191" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A191&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>374</v>
+      </c>
+      <c r="B192" t="s">
+        <v>359</v>
+      </c>
+      <c r="C192" t="s">
+        <v>356</v>
+      </c>
+      <c r="E192" t="s">
+        <v>375</v>
+      </c>
+      <c r="K192" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A192&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>376</v>
+      </c>
+      <c r="B193" t="s">
+        <v>359</v>
+      </c>
+      <c r="C193" t="s">
+        <v>356</v>
+      </c>
+      <c r="E193" t="s">
+        <v>377</v>
+      </c>
+      <c r="K193" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A193&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>378</v>
+      </c>
+      <c r="B194" t="s">
+        <v>65</v>
+      </c>
+      <c r="C194" t="s">
+        <v>356</v>
+      </c>
+      <c r="E194" t="s">
+        <v>377</v>
+      </c>
+      <c r="K194" s="1" t="str">
+        <f>IF(Table2[[#This Row],[Added to RP1]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A194&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
       </c>
     </row>
@@ -5326,7 +5743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5340,7 +5757,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B1" t="str">
         <f>"!PART["&amp;A1&amp;"] {}"</f>
@@ -5349,7 +5766,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B2" t="str">
         <f>"!PART["&amp;A2&amp;"] {}"</f>
@@ -5358,7 +5775,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B3" t="str">
         <f>"!PART["&amp;A3&amp;"] {}"</f>
@@ -5367,11 +5784,179 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B4" t="str">
         <f>"!PART["&amp;A4&amp;"] {}"</f>
         <v>!PART[rn_junoii_sgt_3_dec] {}</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>325</v>
+      </c>
+      <c r="B6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B15" t="s">
+        <v>341</v>
+      </c>
+      <c r="E15" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>329</v>
+      </c>
+      <c r="B16" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>330</v>
+      </c>
+      <c r="B17" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" t="s">
+        <v>343</v>
+      </c>
+      <c r="E18" t="s">
+        <v>344</v>
+      </c>
+      <c r="F18" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>332</v>
+      </c>
+      <c r="B19" t="s">
+        <v>346</v>
+      </c>
+      <c r="E19" t="s">
+        <v>347</v>
+      </c>
+      <c r="F19" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>338</v>
+      </c>
+      <c r="B20" t="s">
+        <v>339</v>
+      </c>
+      <c r="D20" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the Merlin engines to the Patch Manager Removal
</commit_message>
<xml_diff>
--- a/Engine List.xlsx
+++ b/Engine List.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="489">
   <si>
     <t>engineType</t>
   </si>
@@ -467,9 +467,6 @@
     <t>Gamma2</t>
   </si>
   <si>
-    <t>Merlin1</t>
-  </si>
-  <si>
     <t>Falcon 9</t>
   </si>
   <si>
@@ -1467,6 +1464,36 @@
   </si>
   <si>
     <t>Soviet Engines</t>
+  </si>
+  <si>
+    <t>ROE-Merlin1A</t>
+  </si>
+  <si>
+    <t>ROE-Merlin1C</t>
+  </si>
+  <si>
+    <t>ROE-Merlin1CV</t>
+  </si>
+  <si>
+    <t>ROE-Merlin1D</t>
+  </si>
+  <si>
+    <t>ROE-Merlin1DV</t>
+  </si>
+  <si>
+    <t>Merlin1C</t>
+  </si>
+  <si>
+    <t>Merlin1CVac</t>
+  </si>
+  <si>
+    <t>Merlin1D</t>
+  </si>
+  <si>
+    <t>Merlin1DVac</t>
+  </si>
+  <si>
+    <t>Merlin1A</t>
   </si>
 </sst>
 </file>
@@ -1508,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1519,14 +1546,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1573,6 +1610,9 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1678,10 +1718,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P208" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:P208">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P212" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P212">
     <filterColumn colId="11">
-      <filters blank="1"/>
+      <filters>
+        <filter val="ADD"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:O208">
@@ -1700,14 +1742,14 @@
     <tableColumn id="15" name="New PartName" dataDxfId="6">
       <calculatedColumnFormula>IF(I2="","",IF(ISERROR(FIND("-",I2,FIND("-",I2,1)+1)),I2,LEFT(I2,FIND("-",I2,FIND("-",I2,1)+1)-1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="TU Support" dataDxfId="0"/>
-    <tableColumn id="8" name="Complete" dataDxfId="5"/>
-    <tableColumn id="9" name="Added to RP1" dataDxfId="4"/>
-    <tableColumn id="13" name="REMOVE?" dataDxfId="3"/>
-    <tableColumn id="10" name="REMOVE" dataDxfId="2">
+    <tableColumn id="16" name="TU Support" dataDxfId="5"/>
+    <tableColumn id="8" name="Complete" dataDxfId="4"/>
+    <tableColumn id="9" name="Added to RP1" dataDxfId="3"/>
+    <tableColumn id="13" name="REMOVE?" dataDxfId="2"/>
+    <tableColumn id="10" name="REMOVE" dataDxfId="1">
       <calculatedColumnFormula>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A2&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="PatchManager" dataDxfId="1">
+    <tableColumn id="14" name="PatchManager" dataDxfId="0">
       <calculatedColumnFormula>IF(Table2[[#This Row],[REMOVE?]]="X","PatchManager
 {
  modName = ROEngines
@@ -2248,10 +2290,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:P208"/>
+  <dimension ref="A1:P212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="L209" sqref="L209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2289,7 +2331,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>64</v>
@@ -2298,33 +2340,33 @@
         <v>66</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>469</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>304</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
@@ -2345,14 +2387,14 @@
         <v>67</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J2" s="2" t="str">
         <f t="shared" ref="J2:J65" si="0">IF(I2="","",IF(ISERROR(FIND("-",I2,FIND("-",I2,1)+1)),I2,LEFT(I2,FIND("-",I2,FIND("-",I2,1)+1)-1)))</f>
         <v>ROE-A4</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>68</v>
@@ -2411,14 +2453,14 @@
         <v>76</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-Aerobee</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>68</v>
@@ -2456,13 +2498,13 @@
     </row>
     <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
@@ -2471,10 +2513,10 @@
         <v>68</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J4" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2506,13 +2548,13 @@
     </row>
     <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -2521,10 +2563,10 @@
         <v>68</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2554,7 +2596,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -2613,14 +2655,14 @@
         <v>70</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-Agena8048</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>68</v>
@@ -2679,14 +2721,14 @@
         <v>70</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-Agena8096</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>68</v>
@@ -2711,7 +2753,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -2755,7 +2797,7 @@
         <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E10" t="s">
         <v>72</v>
@@ -2767,17 +2809,17 @@
         <v>68</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-AJ10</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>68</v>
@@ -2836,14 +2878,14 @@
         <v>70</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-AJ10</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>68</v>
@@ -2887,7 +2929,7 @@
         <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F12">
         <v>1972</v>
@@ -2896,17 +2938,17 @@
         <v>68</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-AJ10Adv</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>68</v>
@@ -2950,7 +2992,7 @@
         <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F13">
         <v>1959</v>
@@ -2962,14 +3004,14 @@
         <v>67</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-AJ10Early</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>68</v>
@@ -3013,7 +3055,7 @@
         <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F14">
         <v>1960</v>
@@ -3025,14 +3067,14 @@
         <v>67</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-AJ10Mid</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>68</v>
@@ -3070,7 +3112,7 @@
     </row>
     <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B15" t="s">
         <v>31</v>
@@ -3091,7 +3133,7 @@
         <v>32</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3157,7 +3199,7 @@
         <v>32</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3212,7 +3254,7 @@
         <v>32</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3268,7 +3310,7 @@
         <v>32</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J18" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3300,7 +3342,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -3342,7 +3384,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -3384,7 +3426,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -3423,7 +3465,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3465,7 +3507,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -3506,13 +3548,13 @@
     </row>
     <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B24" t="s">
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D24" t="s">
         <v>48</v>
@@ -3527,10 +3569,10 @@
         <v>68</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3575,13 +3617,13 @@
     </row>
     <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B25" t="s">
         <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D25" t="s">
         <v>46</v>
@@ -3596,10 +3638,10 @@
         <v>68</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3650,7 +3692,7 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D26" t="s">
         <v>44</v>
@@ -3665,10 +3707,10 @@
         <v>68</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3711,7 +3753,7 @@
 }</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -3753,7 +3795,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -3798,7 +3840,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -3837,7 +3879,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -3876,7 +3918,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -3917,13 +3959,13 @@
     </row>
     <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E32" t="s">
         <v>84</v>
@@ -3935,10 +3977,10 @@
         <v>68</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J32" s="2" t="str">
         <f t="shared" si="0"/>
@@ -3983,13 +4025,13 @@
     </row>
     <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E33" t="s">
         <v>84</v>
@@ -4001,10 +4043,10 @@
         <v>68</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J33" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4038,13 +4080,13 @@
     </row>
     <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B34" t="s">
         <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E34" t="s">
         <v>84</v>
@@ -4056,10 +4098,10 @@
         <v>68</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J34" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4093,22 +4135,22 @@
     </row>
     <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>336</v>
+      </c>
+      <c r="B35" t="s">
         <v>337</v>
       </c>
-      <c r="B35" t="s">
-        <v>338</v>
-      </c>
       <c r="C35" t="s">
+        <v>334</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I35" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J35" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4149,7 +4191,7 @@
 }</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -4185,7 +4227,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -4218,7 +4260,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>114</v>
       </c>
@@ -4259,7 +4301,7 @@
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E39" t="s">
         <v>113</v>
@@ -4271,10 +4313,10 @@
         <v>68</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J39" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4315,7 +4357,7 @@
 }</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>99</v>
       </c>
@@ -4359,7 +4401,7 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E41" t="s">
         <v>38</v>
@@ -4371,10 +4413,10 @@
         <v>68</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J41" s="2" t="str">
         <f t="shared" si="0"/>
@@ -4415,7 +4457,7 @@
 }</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>104</v>
       </c>
@@ -4448,7 +4490,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -4481,7 +4523,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>101</v>
       </c>
@@ -4517,7 +4559,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -4553,7 +4595,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -4589,7 +4631,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -4625,7 +4667,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -4684,14 +4726,14 @@
         <v>32</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-E1</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>68</v>
@@ -4727,7 +4769,7 @@
 }</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -4792,14 +4834,14 @@
         <v>70</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-F1</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>68</v>
@@ -4835,7 +4877,7 @@
 }</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>90</v>
       </c>
@@ -4871,7 +4913,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>116</v>
       </c>
@@ -4907,7 +4949,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>145</v>
       </c>
@@ -4943,7 +4985,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -4987,7 +5029,7 @@
         <v>31</v>
       </c>
       <c r="C56" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E56" t="s">
         <v>142</v>
@@ -4999,10 +5041,10 @@
         <v>68</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J56" s="2" t="str">
         <f t="shared" si="0"/>
@@ -5043,7 +5085,7 @@
 }</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>140</v>
       </c>
@@ -5082,7 +5124,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>138</v>
       </c>
@@ -5121,7 +5163,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>136</v>
       </c>
@@ -5160,7 +5202,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>134</v>
       </c>
@@ -5196,7 +5238,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>132</v>
       </c>
@@ -5255,14 +5297,14 @@
         <v>70</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J62" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-H1C</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L62" s="1" t="s">
         <v>68</v>
@@ -5321,14 +5363,14 @@
         <v>70</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J63" s="2" t="str">
         <f t="shared" si="0"/>
         <v>ROE-H1D</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L63" s="1" t="s">
         <v>68</v>
@@ -5353,7 +5395,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>129</v>
       </c>
@@ -5386,7 +5428,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>127</v>
       </c>
@@ -5436,14 +5478,14 @@
         <v>70</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J66" s="2" t="str">
         <f t="shared" ref="J66:J129" si="1">IF(I66="","",IF(ISERROR(FIND("-",I66,FIND("-",I66,1)+1)),I66,LEFT(I66,FIND("-",I66,FIND("-",I66,1)+1)-1)))</f>
         <v>ROE-J2</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>68</v>
@@ -5479,7 +5521,7 @@
 }</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>126</v>
       </c>
@@ -5529,14 +5571,14 @@
         <v>70</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J68" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ROE-J2X</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>68</v>
@@ -5572,7 +5614,7 @@
 }</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>123</v>
       </c>
@@ -5611,7 +5653,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>125</v>
       </c>
@@ -5656,7 +5698,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>122</v>
       </c>
@@ -5692,7 +5734,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>120</v>
       </c>
@@ -5728,7 +5770,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>119</v>
       </c>
@@ -5758,7 +5800,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>118</v>
       </c>
@@ -5788,9 +5830,9 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
         <v>63</v>
@@ -5799,7 +5841,7 @@
         <v>67</v>
       </c>
       <c r="E75" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F75">
         <v>1966</v>
@@ -5814,7 +5856,7 @@
       </c>
       <c r="K75" s="2"/>
       <c r="L75" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O75" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A75&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -5833,18 +5875,18 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B76" t="s">
         <v>63</v>
       </c>
       <c r="C76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E76" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I76" s="2"/>
       <c r="J76" s="2" t="str">
@@ -5869,15 +5911,15 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B77" t="s">
         <v>63</v>
       </c>
       <c r="E77" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2" t="str">
@@ -5902,15 +5944,15 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B78" t="s">
         <v>63</v>
       </c>
       <c r="E78" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I78" s="2"/>
       <c r="J78" s="2" t="str">
@@ -5937,25 +5979,25 @@
     </row>
     <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B79" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C79" t="s">
+        <v>334</v>
+      </c>
+      <c r="E79" t="s">
+        <v>347</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H79" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E79" t="s">
-        <v>348</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I79" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J79" s="2" t="str">
         <f t="shared" si="1"/>
@@ -5998,25 +6040,25 @@
     </row>
     <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>435</v>
+      </c>
+      <c r="B80" t="s">
+        <v>337</v>
+      </c>
+      <c r="C80" t="s">
+        <v>334</v>
+      </c>
+      <c r="E80" t="s">
+        <v>347</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I80" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="B80" t="s">
-        <v>338</v>
-      </c>
-      <c r="C80" t="s">
-        <v>335</v>
-      </c>
-      <c r="E80" t="s">
-        <v>348</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>437</v>
       </c>
       <c r="J80" s="2" t="str">
         <f t="shared" si="1"/>
@@ -6047,18 +6089,18 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B81" t="s">
         <v>63</v>
       </c>
       <c r="C81" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>68</v>
@@ -6073,7 +6115,7 @@
       </c>
       <c r="K81" s="2"/>
       <c r="L81" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O81" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A81&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -6092,18 +6134,18 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B82" t="s">
         <v>63</v>
       </c>
       <c r="C82" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E82" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>68</v>
@@ -6118,7 +6160,7 @@
       </c>
       <c r="K82" s="2"/>
       <c r="L82" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O82" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A82&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -6148,7 +6190,7 @@
         <v>32</v>
       </c>
       <c r="E83" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F83">
         <v>1956</v>
@@ -6160,14 +6202,14 @@
         <v>32</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J83" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ROE-LR101</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>68</v>
@@ -6214,7 +6256,7 @@
         <v>32</v>
       </c>
       <c r="E84" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F84">
         <v>1958</v>
@@ -6226,14 +6268,14 @@
         <v>32</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J84" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ROE-LR105</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>68</v>
@@ -6277,10 +6319,10 @@
         <v>63</v>
       </c>
       <c r="C85" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E85" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F85">
         <v>1956</v>
@@ -6289,17 +6331,17 @@
         <v>68</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J85" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ROE-LR79</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>68</v>
@@ -6335,15 +6377,15 @@
 }</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B86" t="s">
         <v>63</v>
       </c>
       <c r="E86" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F86">
         <v>1958</v>
@@ -6373,13 +6415,13 @@
     </row>
     <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B87" t="s">
         <v>63</v>
       </c>
       <c r="E87" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F87">
         <v>1959</v>
@@ -6388,10 +6430,10 @@
         <v>68</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J87" s="2" t="str">
         <f t="shared" si="1"/>
@@ -6432,9 +6474,9 @@
 }</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B88" t="s">
         <v>63</v>
@@ -6476,7 +6518,7 @@
         <v>32</v>
       </c>
       <c r="E89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F89">
         <v>1958</v>
@@ -6488,14 +6530,14 @@
         <v>32</v>
       </c>
       <c r="I89" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J89" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ROE-LR89</v>
       </c>
       <c r="K89" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L89" s="1" t="s">
         <v>68</v>
@@ -6533,13 +6575,13 @@
     </row>
     <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B90" t="s">
         <v>63</v>
       </c>
       <c r="E90" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F90">
         <v>1959</v>
@@ -6548,10 +6590,10 @@
         <v>68</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J90" s="2" t="str">
         <f t="shared" si="1"/>
@@ -6594,7 +6636,7 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B91" t="s">
         <v>63</v>
@@ -6614,6 +6656,9 @@
         <v/>
       </c>
       <c r="K91" s="2"/>
+      <c r="L91" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="O91" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A91&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
         <v/>
@@ -6631,15 +6676,15 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B92" t="s">
         <v>31</v>
       </c>
       <c r="E92" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F92">
         <v>1962</v>
@@ -6669,7 +6714,7 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>146</v>
+        <v>488</v>
       </c>
       <c r="B93" t="s">
         <v>63</v>
@@ -6678,7 +6723,7 @@
         <v>70</v>
       </c>
       <c r="E93" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F93">
         <v>2006</v>
@@ -6689,15 +6734,28 @@
       <c r="H93" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I93" s="2"/>
+      <c r="I93" s="2" t="s">
+        <v>479</v>
+      </c>
       <c r="J93" s="2" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K93" s="2"/>
+        <v>ROE-Merlin1A</v>
+      </c>
+      <c r="K93" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N93" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="O93" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A93&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
-        <v/>
+        <v>!PART:HAS[~name[ROE-*]&amp;#engineType[Merlin1A]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}</v>
       </c>
       <c r="P93" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","PatchManager
@@ -6709,18 +6767,26 @@
  longDescr = Removes the duplicated "&amp;Table2[[#This Row],[Engine]]&amp;" engines from other mods.
  installedWithMod = True
 }","")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+        <v>PatchManager
+{
+ modName = ROEngines
+ srcPath = ROEngines/PatchManager/PluginData/Merlin1A.cfg
+ patchName = Merlin1A
+ shortDescr = Merlin1A
+ longDescr = Removes the duplicated Merlin1A engines from other mods.
+ installedWithMod = True
+}</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B94" t="s">
         <v>63</v>
       </c>
       <c r="E94" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I94" s="2"/>
       <c r="J94" s="2" t="str">
@@ -6747,25 +6813,25 @@
     </row>
     <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B95" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C95" t="s">
+        <v>334</v>
+      </c>
+      <c r="E95" t="s">
+        <v>340</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H95" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E95" t="s">
-        <v>341</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I95" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J95" s="2" t="str">
         <f t="shared" si="1"/>
@@ -6796,15 +6862,15 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B96" t="s">
         <v>63</v>
       </c>
       <c r="E96" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2" t="str">
@@ -6829,15 +6895,15 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B97" t="s">
         <v>63</v>
       </c>
       <c r="E97" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="2" t="str">
@@ -6862,15 +6928,15 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
         <v>63</v>
       </c>
       <c r="E98" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I98" s="2"/>
       <c r="J98" s="2" t="str">
@@ -6906,7 +6972,7 @@
         <v>67</v>
       </c>
       <c r="E99" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F99">
         <v>1952</v>
@@ -6918,7 +6984,7 @@
         <v>67</v>
       </c>
       <c r="I99" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J99" s="2" t="str">
         <f t="shared" si="1"/>
@@ -6959,9 +7025,9 @@
 }</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B100" t="s">
         <v>79</v>
@@ -6989,9 +7055,9 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B101" t="s">
         <v>79</v>
@@ -7019,9 +7085,9 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B102" t="s">
         <v>79</v>
@@ -7049,9 +7115,9 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B103" t="s">
         <v>79</v>
@@ -7081,16 +7147,16 @@
     </row>
     <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B104" t="s">
         <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E104" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F104">
         <v>1955</v>
@@ -7099,10 +7165,10 @@
         <v>68</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I104" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J104" s="2" t="str">
         <f t="shared" si="1"/>
@@ -7145,7 +7211,7 @@
     </row>
     <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B105" t="s">
         <v>63</v>
@@ -7154,7 +7220,7 @@
         <v>67</v>
       </c>
       <c r="E105" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>68</v>
@@ -7163,7 +7229,7 @@
         <v>67</v>
       </c>
       <c r="I105" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J105" s="2" t="str">
         <f t="shared" si="1"/>
@@ -7206,7 +7272,7 @@
     </row>
     <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B106" t="s">
         <v>63</v>
@@ -7215,7 +7281,7 @@
         <v>67</v>
       </c>
       <c r="E106" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>68</v>
@@ -7224,7 +7290,7 @@
         <v>67</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J106" s="2" t="str">
         <f t="shared" si="1"/>
@@ -7265,15 +7331,15 @@
 }</v>
       </c>
     </row>
-    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B107" t="s">
         <v>63</v>
       </c>
       <c r="E107" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>68</v>
@@ -7288,7 +7354,7 @@
       </c>
       <c r="K107" s="2"/>
       <c r="L107" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O107" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A107&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -7307,15 +7373,15 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B108" t="s">
         <v>63</v>
       </c>
       <c r="E108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>68</v>
@@ -7330,7 +7396,7 @@
       </c>
       <c r="K108" s="2"/>
       <c r="L108" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O108" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A108&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -7349,12 +7415,12 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>208</v>
+      </c>
+      <c r="B109" t="s">
         <v>209</v>
-      </c>
-      <c r="B109" t="s">
-        <v>210</v>
       </c>
       <c r="I109" s="2"/>
       <c r="J109" s="2" t="str">
@@ -7379,9 +7445,9 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B110" t="s">
         <v>79</v>
@@ -7409,9 +7475,9 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B111" t="s">
         <v>79</v>
@@ -7439,9 +7505,9 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B112" t="s">
         <v>79</v>
@@ -7471,16 +7537,16 @@
     </row>
     <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B113" t="s">
         <v>63</v>
       </c>
       <c r="C113" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D113" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E113" t="s">
         <v>71</v>
@@ -7489,10 +7555,10 @@
         <v>68</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I113" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J113" s="2" t="str">
         <f t="shared" si="1"/>
@@ -7524,25 +7590,25 @@
     </row>
     <row r="114" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B114" t="s">
         <v>63</v>
       </c>
       <c r="C114" t="s">
+        <v>334</v>
+      </c>
+      <c r="E114" t="s">
+        <v>333</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H114" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E114" t="s">
-        <v>334</v>
-      </c>
-      <c r="G114" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I114" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J114" s="2" t="str">
         <f t="shared" si="1"/>
@@ -7574,25 +7640,25 @@
     </row>
     <row r="115" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B115" t="s">
         <v>63</v>
       </c>
       <c r="C115" t="s">
+        <v>334</v>
+      </c>
+      <c r="E115" t="s">
+        <v>347</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H115" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E115" t="s">
-        <v>348</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I115" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J115" s="2" t="str">
         <f t="shared" si="1"/>
@@ -7633,9 +7699,9 @@
 }</v>
       </c>
     </row>
-    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B116" t="s">
         <v>63</v>
@@ -7644,7 +7710,7 @@
         <v>67</v>
       </c>
       <c r="E116" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>68</v>
@@ -7659,7 +7725,7 @@
       </c>
       <c r="K116" s="2"/>
       <c r="L116" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O116" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A116&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -7680,32 +7746,32 @@
     </row>
     <row r="117" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B117" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C117" t="s">
+        <v>334</v>
+      </c>
+      <c r="E117" t="s">
+        <v>342</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H117" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E117" t="s">
-        <v>343</v>
-      </c>
-      <c r="G117" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H117" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I117" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J117" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ROE-MR104</v>
       </c>
       <c r="K117" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L117" s="1" t="s">
         <v>68</v>
@@ -7732,29 +7798,29 @@
     </row>
     <row r="118" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>448</v>
+      </c>
+      <c r="B118" t="s">
+        <v>337</v>
+      </c>
+      <c r="C118" t="s">
+        <v>334</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I118" s="2" t="s">
         <v>449</v>
-      </c>
-      <c r="B118" t="s">
-        <v>338</v>
-      </c>
-      <c r="C118" t="s">
-        <v>335</v>
-      </c>
-      <c r="G118" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H118" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="I118" s="2" t="s">
-        <v>450</v>
       </c>
       <c r="J118" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ROE-PLE</v>
       </c>
       <c r="K118" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L118" s="1" t="s">
         <v>68</v>
@@ -7781,29 +7847,29 @@
     </row>
     <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>442</v>
+      </c>
+      <c r="B119" t="s">
+        <v>337</v>
+      </c>
+      <c r="C119" t="s">
+        <v>334</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I119" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="B119" t="s">
-        <v>338</v>
-      </c>
-      <c r="C119" t="s">
-        <v>335</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H119" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="I119" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="J119" s="2" t="str">
         <f t="shared" si="1"/>
         <v>ROE-S400</v>
       </c>
       <c r="K119" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L119" s="1" t="s">
         <v>68</v>
@@ -7830,13 +7896,13 @@
     </row>
     <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B120" t="s">
         <v>63</v>
       </c>
       <c r="E120" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F120">
         <v>1958</v>
@@ -7845,10 +7911,10 @@
         <v>68</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J120" s="2" t="str">
         <f t="shared" si="1"/>
@@ -7883,7 +7949,7 @@
         <v>63</v>
       </c>
       <c r="E121" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F121">
         <v>1960</v>
@@ -7895,7 +7961,7 @@
         <v>70</v>
       </c>
       <c r="I121" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J121" s="2" t="str">
         <f t="shared" si="1"/>
@@ -7936,18 +8002,18 @@
 }</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B122" t="s">
         <v>63</v>
       </c>
       <c r="D122" t="s">
+        <v>190</v>
+      </c>
+      <c r="E122" t="s">
         <v>191</v>
-      </c>
-      <c r="E122" t="s">
-        <v>192</v>
       </c>
       <c r="F122">
         <v>2013</v>
@@ -7975,18 +8041,18 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B123" t="s">
         <v>63</v>
       </c>
       <c r="D123" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E123" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F123">
         <v>2013</v>
@@ -8014,15 +8080,15 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B124" t="s">
         <v>63</v>
       </c>
       <c r="E124" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>68</v>
@@ -8037,7 +8103,7 @@
       </c>
       <c r="K124" s="2"/>
       <c r="L124" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O124" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A124&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8056,15 +8122,15 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B125" t="s">
         <v>63</v>
       </c>
       <c r="E125" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>67</v>
@@ -8076,7 +8142,7 @@
       </c>
       <c r="K125" s="2"/>
       <c r="L125" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O125" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A125&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8095,15 +8161,15 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B126" t="s">
         <v>63</v>
       </c>
       <c r="D126" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>67</v>
@@ -8115,7 +8181,7 @@
       </c>
       <c r="K126" s="2"/>
       <c r="L126" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O126" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A126&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8134,15 +8200,15 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B127" t="s">
         <v>63</v>
       </c>
       <c r="E127" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>67</v>
@@ -8154,7 +8220,7 @@
       </c>
       <c r="K127" s="2"/>
       <c r="L127" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O127" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A127&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8173,15 +8239,15 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B128" t="s">
         <v>63</v>
       </c>
       <c r="E128" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>67</v>
@@ -8193,7 +8259,7 @@
       </c>
       <c r="K128" s="2"/>
       <c r="L128" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O128" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A128&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8212,15 +8278,15 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B129" t="s">
         <v>63</v>
       </c>
       <c r="E129" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I129" s="2"/>
       <c r="J129" s="2" t="str">
@@ -8245,18 +8311,18 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B130" t="s">
         <v>63</v>
       </c>
       <c r="D130" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E130" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I130" s="2"/>
       <c r="J130" s="2" t="str">
@@ -8281,9 +8347,9 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B131" t="s">
         <v>63</v>
@@ -8311,9 +8377,9 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B132" t="s">
         <v>79</v>
@@ -8361,7 +8427,7 @@
         <v>67</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J133" s="2" t="str">
         <f t="shared" si="2"/>
@@ -8413,7 +8479,7 @@
         <v>70</v>
       </c>
       <c r="E134" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F134">
         <v>1956</v>
@@ -8425,14 +8491,14 @@
         <v>70</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J134" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RD107</v>
       </c>
       <c r="K134" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L134" s="1" t="s">
         <v>68</v>
@@ -8479,7 +8545,7 @@
         <v>70</v>
       </c>
       <c r="E135" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F135">
         <v>1956</v>
@@ -8491,14 +8557,14 @@
         <v>70</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J135" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RD108</v>
       </c>
       <c r="K135" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L135" s="1" t="s">
         <v>68</v>
@@ -8534,15 +8600,15 @@
 }</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B136" t="s">
         <v>63</v>
       </c>
       <c r="E136" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I136" s="2"/>
       <c r="J136" s="2" t="str">
@@ -8578,7 +8644,7 @@
         <v>70</v>
       </c>
       <c r="E137" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>68</v>
@@ -8587,14 +8653,14 @@
         <v>70</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J137" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RD170</v>
       </c>
       <c r="K137" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L137" s="1" t="s">
         <v>68</v>
@@ -8650,14 +8716,14 @@
         <v>70</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J138" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RD180</v>
       </c>
       <c r="K138" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L138" s="1" t="s">
         <v>68</v>
@@ -8704,7 +8770,7 @@
         <v>70</v>
       </c>
       <c r="E139" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>68</v>
@@ -8713,14 +8779,14 @@
         <v>70</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J139" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RD191</v>
       </c>
       <c r="K139" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L139" s="1" t="s">
         <v>68</v>
@@ -8756,15 +8822,15 @@
 }</v>
       </c>
     </row>
-    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B140" t="s">
         <v>63</v>
       </c>
       <c r="E140" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>67</v>
@@ -8776,7 +8842,7 @@
       </c>
       <c r="K140" s="2"/>
       <c r="L140" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O140" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A140&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8795,18 +8861,18 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B141" t="s">
         <v>63</v>
       </c>
       <c r="D141" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I141" s="2"/>
       <c r="J141" s="2" t="str">
@@ -8815,7 +8881,7 @@
       </c>
       <c r="K141" s="2"/>
       <c r="L141" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O141" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A141&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8834,18 +8900,18 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B142" t="s">
         <v>63</v>
       </c>
       <c r="E142" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I142" s="2"/>
       <c r="J142" s="2" t="str">
@@ -8854,7 +8920,7 @@
       </c>
       <c r="K142" s="2"/>
       <c r="L142" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O142" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A142&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8873,15 +8939,15 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B143" t="s">
         <v>63</v>
       </c>
       <c r="E143" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I143" s="2"/>
       <c r="J143" s="2" t="str">
@@ -8890,7 +8956,7 @@
       </c>
       <c r="K143" s="2"/>
       <c r="L143" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O143" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A143&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -8911,13 +8977,13 @@
     </row>
     <row r="144" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B144" t="s">
         <v>63</v>
       </c>
       <c r="E144" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>68</v>
@@ -8926,7 +8992,7 @@
         <v>67</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J144" s="2" t="str">
         <f t="shared" si="2"/>
@@ -8967,15 +9033,15 @@
 }</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B145" t="s">
         <v>63</v>
       </c>
       <c r="E145" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I145" s="2"/>
       <c r="J145" s="2" t="str">
@@ -9000,15 +9066,15 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B146" t="s">
         <v>63</v>
       </c>
       <c r="E146" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I146" s="2"/>
       <c r="J146" s="2" t="str">
@@ -9035,16 +9101,16 @@
     </row>
     <row r="147" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B147" t="s">
         <v>63</v>
       </c>
       <c r="D147" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E147" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>68</v>
@@ -9053,7 +9119,7 @@
         <v>67</v>
       </c>
       <c r="I147" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J147" s="2" t="str">
         <f t="shared" si="2"/>
@@ -9094,15 +9160,15 @@
 }</v>
       </c>
     </row>
-    <row r="148" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B148" t="s">
         <v>63</v>
       </c>
       <c r="E148" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>67</v>
@@ -9114,7 +9180,7 @@
       </c>
       <c r="K148" s="2"/>
       <c r="L148" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O148" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A148&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -9133,18 +9199,18 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B149" t="s">
         <v>63</v>
       </c>
       <c r="D149" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E149" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F149">
         <v>1964</v>
@@ -9172,18 +9238,18 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B150" t="s">
         <v>63</v>
       </c>
       <c r="D150" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E150" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F150">
         <v>1964</v>
@@ -9198,7 +9264,7 @@
       </c>
       <c r="K150" s="2"/>
       <c r="L150" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O150" s="1" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A150&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
@@ -9217,9 +9283,9 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B151" t="s">
         <v>31</v>
@@ -9267,7 +9333,7 @@
         <v>70</v>
       </c>
       <c r="E152" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>68</v>
@@ -9276,14 +9342,14 @@
         <v>70</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J152" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RL10A3</v>
       </c>
       <c r="K152" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L152" s="1" t="s">
         <v>68</v>
@@ -9330,7 +9396,7 @@
         <v>70</v>
       </c>
       <c r="E153" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G153" s="1" t="s">
         <v>68</v>
@@ -9339,14 +9405,14 @@
         <v>70</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J153" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RL10A3</v>
       </c>
       <c r="K153" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L153" s="1" t="s">
         <v>68</v>
@@ -9382,7 +9448,7 @@
         <v>70</v>
       </c>
       <c r="E154" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>68</v>
@@ -9391,14 +9457,14 @@
         <v>70</v>
       </c>
       <c r="I154" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J154" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RL10A5</v>
       </c>
       <c r="K154" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>68</v>
@@ -9434,7 +9500,7 @@
         <v>70</v>
       </c>
       <c r="E155" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>68</v>
@@ -9443,14 +9509,14 @@
         <v>70</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J155" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RL10B2</v>
       </c>
       <c r="K155" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L155" s="1" t="s">
         <v>68</v>
@@ -9475,15 +9541,15 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B156" t="s">
         <v>63</v>
       </c>
       <c r="E156" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I156" s="2"/>
       <c r="J156" s="2" t="str">
@@ -9528,14 +9594,14 @@
         <v>70</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J157" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RS68</v>
       </c>
       <c r="K157" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>68</v>
@@ -9571,15 +9637,15 @@
 }</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B158" t="s">
         <v>63</v>
       </c>
       <c r="E158" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I158" s="2"/>
       <c r="J158" s="2" t="str">
@@ -9604,9 +9670,9 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B159" t="s">
         <v>31</v>
@@ -9643,15 +9709,15 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B160" t="s">
         <v>31</v>
       </c>
       <c r="E160" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F160">
         <v>2012</v>
@@ -9679,9 +9745,9 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B161" t="s">
         <v>31</v>
@@ -9720,22 +9786,22 @@
     </row>
     <row r="162" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B162" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C162" t="s">
+        <v>334</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H162" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="G162" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H162" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I162" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J162" s="2" t="str">
         <f t="shared" si="2"/>
@@ -9778,22 +9844,22 @@
     </row>
     <row r="163" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B163" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C163" t="s">
+        <v>334</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H163" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="G163" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H163" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I163" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J163" s="2" t="str">
         <f t="shared" si="2"/>
@@ -9826,16 +9892,16 @@
     </row>
     <row r="164" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B164" t="s">
         <v>63</v>
       </c>
       <c r="C164" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E164" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F164">
         <v>1953</v>
@@ -9844,10 +9910,10 @@
         <v>68</v>
       </c>
       <c r="H164" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="I164" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="I164" s="2" t="s">
-        <v>460</v>
       </c>
       <c r="J164" s="2" t="str">
         <f t="shared" si="2"/>
@@ -9890,16 +9956,16 @@
     </row>
     <row r="165" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B165" t="s">
         <v>63</v>
       </c>
       <c r="C165" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E165" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F165">
         <v>2000</v>
@@ -9908,14 +9974,14 @@
         <v>68</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J165" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-S592</v>
       </c>
       <c r="K165" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="L165" s="1" t="s">
         <v>68</v>
@@ -9953,16 +10019,16 @@
     </row>
     <row r="166" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B166" t="s">
         <v>63</v>
       </c>
       <c r="C166" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E166" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F166">
         <v>2000</v>
@@ -9971,10 +10037,10 @@
         <v>68</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J166" s="2" t="str">
         <f t="shared" si="2"/>
@@ -10015,15 +10081,15 @@
 }</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B167" t="s">
         <v>63</v>
       </c>
       <c r="D167" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E167" t="s">
         <v>92</v>
@@ -10054,9 +10120,9 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B168" t="s">
         <v>79</v>
@@ -10084,15 +10150,15 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B169" t="s">
         <v>31</v>
       </c>
       <c r="E169" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F169">
         <v>1989</v>
@@ -10143,14 +10209,14 @@
         <v>70</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J170" s="2" t="str">
         <f t="shared" si="2"/>
         <v>ROE-RS25</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L170" s="1" t="s">
         <v>68</v>
@@ -10186,9 +10252,9 @@
 }</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B171" t="s">
         <v>31</v>
@@ -10216,9 +10282,9 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B172" t="s">
         <v>31</v>
@@ -10246,9 +10312,9 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B173" t="s">
         <v>31</v>
@@ -10279,9 +10345,9 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B174" t="s">
         <v>31</v>
@@ -10309,9 +10375,9 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B175" t="s">
         <v>31</v>
@@ -10339,9 +10405,9 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B176" t="s">
         <v>31</v>
@@ -10369,9 +10435,9 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B177" t="s">
         <v>31</v>
@@ -10399,9 +10465,9 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B178" t="s">
         <v>31</v>
@@ -10429,9 +10495,9 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B179" t="s">
         <v>31</v>
@@ -10459,9 +10525,9 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B180" t="s">
         <v>31</v>
@@ -10489,9 +10555,9 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B181" t="s">
         <v>31</v>
@@ -10522,9 +10588,9 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B182" t="s">
         <v>31</v>
@@ -10555,9 +10621,9 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B183" t="s">
         <v>31</v>
@@ -10588,9 +10654,9 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B184" t="s">
         <v>31</v>
@@ -10621,9 +10687,9 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B185" t="s">
         <v>31</v>
@@ -10654,9 +10720,9 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B186" t="s">
         <v>31</v>
@@ -10689,25 +10755,25 @@
     </row>
     <row r="187" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>343</v>
+      </c>
+      <c r="B187" t="s">
+        <v>337</v>
+      </c>
+      <c r="C187" t="s">
+        <v>334</v>
+      </c>
+      <c r="E187" t="s">
         <v>344</v>
       </c>
-      <c r="B187" t="s">
-        <v>338</v>
-      </c>
-      <c r="C187" t="s">
+      <c r="G187" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H187" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E187" t="s">
-        <v>345</v>
-      </c>
-      <c r="G187" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H187" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I187" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J187" s="2" t="str">
         <f t="shared" si="2"/>
@@ -10748,9 +10814,9 @@
 }</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B188" t="s">
         <v>31</v>
@@ -10781,9 +10847,9 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B189" t="s">
         <v>31</v>
@@ -10816,25 +10882,25 @@
     </row>
     <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>345</v>
+      </c>
+      <c r="B190" t="s">
+        <v>337</v>
+      </c>
+      <c r="C190" t="s">
+        <v>334</v>
+      </c>
+      <c r="E190" t="s">
         <v>346</v>
       </c>
-      <c r="B190" t="s">
-        <v>338</v>
-      </c>
-      <c r="C190" t="s">
+      <c r="G190" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H190" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E190" t="s">
-        <v>347</v>
-      </c>
-      <c r="G190" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H190" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I190" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J190" s="2" t="str">
         <f t="shared" si="2"/>
@@ -10875,9 +10941,9 @@
 }</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B191" t="s">
         <v>31</v>
@@ -10910,25 +10976,25 @@
     </row>
     <row r="192" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B192" t="s">
         <v>63</v>
       </c>
       <c r="C192" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E192" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G192" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I192" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J192" s="2" t="str">
         <f t="shared" si="2"/>
@@ -10960,25 +11026,25 @@
     </row>
     <row r="193" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B193" t="s">
         <v>63</v>
       </c>
       <c r="C193" t="s">
+        <v>334</v>
+      </c>
+      <c r="E193" t="s">
+        <v>300</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H193" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E193" t="s">
-        <v>301</v>
-      </c>
-      <c r="G193" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H193" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I193" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J193" s="2" t="str">
         <f t="shared" si="2"/>
@@ -11010,25 +11076,25 @@
     </row>
     <row r="194" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B194" t="s">
         <v>63</v>
       </c>
       <c r="E194" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G194" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I194" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J194" s="2" t="str">
-        <f t="shared" ref="J194:J257" si="3">IF(I194="","",IF(ISERROR(FIND("-",I194,FIND("-",I194,1)+1)),I194,LEFT(I194,FIND("-",I194,FIND("-",I194,1)+1)-1)))</f>
+        <f t="shared" ref="J194:J212" si="3">IF(I194="","",IF(ISERROR(FIND("-",I194,FIND("-",I194,1)+1)),I194,LEFT(I194,FIND("-",I194,FIND("-",I194,1)+1)-1)))</f>
         <v>ROE-TD339</v>
       </c>
       <c r="K194" s="2"/>
@@ -11068,25 +11134,25 @@
     </row>
     <row r="195" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B195" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C195" t="s">
+        <v>334</v>
+      </c>
+      <c r="E195" t="s">
+        <v>341</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H195" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E195" t="s">
-        <v>342</v>
-      </c>
-      <c r="G195" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H195" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="I195" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J195" s="2" t="str">
         <f t="shared" si="3"/>
@@ -11127,9 +11193,9 @@
 }</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B196" t="s">
         <v>31</v>
@@ -11163,15 +11229,15 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B197" t="s">
         <v>31</v>
       </c>
       <c r="E197" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F197">
         <v>1965</v>
@@ -11202,15 +11268,15 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B198" t="s">
         <v>31</v>
       </c>
       <c r="E198" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F198">
         <v>1989</v>
@@ -11241,9 +11307,9 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B199" t="s">
         <v>63</v>
@@ -11277,15 +11343,15 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B200" t="s">
         <v>63</v>
       </c>
       <c r="E200" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I200" s="2"/>
       <c r="J200" s="2" t="str">
@@ -11310,15 +11376,15 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B201" t="s">
         <v>63</v>
       </c>
       <c r="E201" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I201" s="2"/>
       <c r="J201" s="2" t="str">
@@ -11343,9 +11409,9 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B202" t="s">
         <v>31</v>
@@ -11381,13 +11447,13 @@
     </row>
     <row r="203" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B203" t="s">
         <v>63</v>
       </c>
       <c r="C203" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E203" t="s">
         <v>142</v>
@@ -11402,14 +11468,14 @@
         <v>32</v>
       </c>
       <c r="I203" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J203" s="2" t="str">
         <f t="shared" si="3"/>
         <v>ROE-X405</v>
       </c>
       <c r="K203" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L203" s="1" t="s">
         <v>68</v>
@@ -11447,7 +11513,7 @@
     </row>
     <row r="204" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B204" t="s">
         <v>63</v>
@@ -11456,7 +11522,7 @@
         <v>32</v>
       </c>
       <c r="E204" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>68</v>
@@ -11465,14 +11531,14 @@
         <v>32</v>
       </c>
       <c r="I204" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J204" s="2" t="str">
         <f t="shared" si="3"/>
         <v>ROE-X405H</v>
       </c>
       <c r="K204" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L204" s="1" t="s">
         <v>68</v>
@@ -11508,12 +11574,12 @@
 }</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B205" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I205" s="2"/>
       <c r="J205" s="2" t="str">
@@ -11538,15 +11604,15 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B206" t="s">
         <v>63</v>
       </c>
       <c r="E206" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F206">
         <v>0</v>
@@ -11574,15 +11640,15 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B207" t="s">
         <v>63</v>
       </c>
       <c r="E207" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F207">
         <v>1959</v>
@@ -11610,15 +11676,15 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B208" t="s">
         <v>63</v>
       </c>
       <c r="E208" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I208" s="2"/>
       <c r="J208" s="2" t="str">
@@ -11631,6 +11697,234 @@
         <v/>
       </c>
       <c r="P208" s="1" t="str">
+        <f>IF(Table2[[#This Row],[REMOVE?]]="X","PatchManager
+{
+ modName = ROEngines
+ srcPath = ROEngines/PatchManager/PluginData/"&amp;Table2[[#This Row],[Engine]]&amp;".cfg
+ patchName = "&amp;Table2[[#This Row],[Engine]]&amp;"
+ shortDescr = "&amp;Table2[[#This Row],[Engine]]&amp;"
+ longDescr = Removes the duplicated "&amp;Table2[[#This Row],[Engine]]&amp;" engines from other mods.
+ installedWithMod = True
+}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A209" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D209" s="4"/>
+      <c r="E209" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F209" s="4">
+        <v>2006</v>
+      </c>
+      <c r="G209" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H209" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I209" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="J209" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>ROE-Merlin1C</v>
+      </c>
+      <c r="K209" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="L209" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M209" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N209" s="5"/>
+      <c r="O209" s="8" t="str">
+        <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A209&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+      <c r="P209" s="8" t="str">
+        <f>IF(Table2[[#This Row],[REMOVE?]]="X","PatchManager
+{
+ modName = ROEngines
+ srcPath = ROEngines/PatchManager/PluginData/"&amp;Table2[[#This Row],[Engine]]&amp;".cfg
+ patchName = "&amp;Table2[[#This Row],[Engine]]&amp;"
+ shortDescr = "&amp;Table2[[#This Row],[Engine]]&amp;"
+ longDescr = Removes the duplicated "&amp;Table2[[#This Row],[Engine]]&amp;" engines from other mods.
+ installedWithMod = True
+}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A210" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D210" s="4"/>
+      <c r="E210" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F210" s="4">
+        <v>2006</v>
+      </c>
+      <c r="G210" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H210" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I210" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="J210" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>ROE-Merlin1CV</v>
+      </c>
+      <c r="K210" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="L210" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M210" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N210" s="5"/>
+      <c r="O210" s="8" t="str">
+        <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A210&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+      <c r="P210" s="8" t="str">
+        <f>IF(Table2[[#This Row],[REMOVE?]]="X","PatchManager
+{
+ modName = ROEngines
+ srcPath = ROEngines/PatchManager/PluginData/"&amp;Table2[[#This Row],[Engine]]&amp;".cfg
+ patchName = "&amp;Table2[[#This Row],[Engine]]&amp;"
+ shortDescr = "&amp;Table2[[#This Row],[Engine]]&amp;"
+ longDescr = Removes the duplicated "&amp;Table2[[#This Row],[Engine]]&amp;" engines from other mods.
+ installedWithMod = True
+}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A211" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D211" s="4"/>
+      <c r="E211" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F211" s="4">
+        <v>2006</v>
+      </c>
+      <c r="G211" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H211" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I211" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="J211" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>ROE-Merlin1D</v>
+      </c>
+      <c r="K211" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="L211" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M211" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N211" s="5"/>
+      <c r="O211" s="8" t="str">
+        <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A211&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+      <c r="P211" s="8" t="str">
+        <f>IF(Table2[[#This Row],[REMOVE?]]="X","PatchManager
+{
+ modName = ROEngines
+ srcPath = ROEngines/PatchManager/PluginData/"&amp;Table2[[#This Row],[Engine]]&amp;".cfg
+ patchName = "&amp;Table2[[#This Row],[Engine]]&amp;"
+ shortDescr = "&amp;Table2[[#This Row],[Engine]]&amp;"
+ longDescr = Removes the duplicated "&amp;Table2[[#This Row],[Engine]]&amp;" engines from other mods.
+ installedWithMod = True
+}","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A212" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D212" s="4"/>
+      <c r="E212" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F212" s="4">
+        <v>2006</v>
+      </c>
+      <c r="G212" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H212" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I212" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="J212" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>ROE-Merlin1DV</v>
+      </c>
+      <c r="K212" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="L212" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M212" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N212" s="5"/>
+      <c r="O212" s="8" t="str">
+        <f>IF(Table2[[#This Row],[REMOVE?]]="X","!PART:HAS[~name[ROE-*]&amp;#engineType["&amp;A212&amp;"]&amp;#category[Engine]]:BEFORE[zzzTagCleanup] {}","")</f>
+        <v/>
+      </c>
+      <c r="P212" s="8" t="str">
         <f>IF(Table2[[#This Row],[REMOVE?]]="X","PatchManager
 {
  modName = ROEngines
@@ -11668,7 +11962,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B1" t="str">
         <f>"!PART["&amp;A1&amp;"] {}"</f>
@@ -11677,7 +11971,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B2" t="str">
         <f>"!PART["&amp;A2&amp;"] {}"</f>
@@ -11686,7 +11980,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B3" t="str">
         <f>"!PART["&amp;A3&amp;"] {}"</f>
@@ -11695,7 +11989,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B4" t="str">
         <f>"!PART["&amp;A4&amp;"] {}"</f>
@@ -11733,24 +12027,24 @@
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K2" t="s">
+        <v>423</v>
+      </c>
+      <c r="L2" t="s">
         <v>424</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>425</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>426</v>
-      </c>
-      <c r="N2" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J3" s="1">
         <v>4</v>
@@ -11771,7 +12065,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J4" s="1">
         <v>5</v>
@@ -11796,7 +12090,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J5" s="1">
         <v>6</v>
@@ -11821,7 +12115,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J6" s="1">
         <v>7</v>
@@ -11842,13 +12136,13 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J8">
         <v>3.35</v>
       </c>
       <c r="M8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="N8">
         <v>3.048</v>
@@ -11856,7 +12150,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="N9">
         <v>8.5299999999999994</v>
@@ -11864,68 +12158,68 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B15" t="s">
+        <v>322</v>
+      </c>
+      <c r="E15" t="s">
         <v>323</v>
-      </c>
-      <c r="E15" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B18" t="s">
+        <v>324</v>
+      </c>
+      <c r="E18" t="s">
         <v>325</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>326</v>
-      </c>
-      <c r="F18" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B19" t="s">
+        <v>327</v>
+      </c>
+      <c r="E19" t="s">
         <v>328</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>329</v>
-      </c>
-      <c r="F19" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>319</v>
+      </c>
+      <c r="B20" t="s">
         <v>320</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>321</v>
-      </c>
-      <c r="D20" t="s">
-        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>